<commit_message>
Relabeled incorrect images in cropped_images_labelled and the excel
</commit_message>
<xml_diff>
--- a/Annotated_Emotion_Data.xlsx
+++ b/Annotated_Emotion_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alvaro Millan Ruiz\Desktop\dsp_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72423676-3945-4136-9326-0BF55F10D6F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C0185F-F817-44C0-8A0C-A189D93182A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1191" uniqueCount="778">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1193" uniqueCount="779">
   <si>
     <t>https://lh4.ggpht.com/RcottnlLRe9AZBQe8H1U-_2sbesuVL5lksBhPszE47-eLrIzrbX5cUNzhsVlDDbIYiqL2jR0wWx82FKQA5YN50h_tlw=s0</t>
   </si>
@@ -2367,13 +2367,16 @@
   </si>
   <si>
     <t>Comparison</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2516,8 +2519,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2697,8 +2706,14 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -2828,6 +2843,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2874,7 +2902,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2886,6 +2914,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="42" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2932,7 +2968,144 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="10"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2974,6 +3147,23 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2496DF01-8E1F-4C3F-B53D-20267B8104CE}" name="Table2" displayName="Table2" ref="A1:H768" totalsRowCount="1" headerRowDxfId="4" headerRowBorderDxfId="3" tableBorderDxfId="2">
+  <autoFilter ref="A1:H767" xr:uid="{2496DF01-8E1F-4C3F-B53D-20267B8104CE}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{0AB31B11-92D5-429B-96D5-08A6F799CE69}" name="Image URL" totalsRowLabel="Total" dataDxfId="1" totalsRowDxfId="0" dataCellStyle="Hyperlink"/>
+    <tableColumn id="2" xr3:uid="{E6E63F4D-86A8-4399-B758-1AD3EE22553B}" name="Angry" totalsRowFunction="count"/>
+    <tableColumn id="3" xr3:uid="{D3123506-717E-4294-8881-AB2CFFAAF65A}" name="Sad " totalsRowFunction="count"/>
+    <tableColumn id="4" xr3:uid="{21511BB0-C242-410A-A2ED-9EEA0891B1E7}" name="Happy" totalsRowFunction="count"/>
+    <tableColumn id="5" xr3:uid="{D97D38C8-27B2-4905-B806-17038F792BB3}" name="Fear" totalsRowFunction="count"/>
+    <tableColumn id="6" xr3:uid="{96E5A548-BF3F-4A97-89A3-A63A6FFD9966}" name="Surprise" totalsRowFunction="count"/>
+    <tableColumn id="7" xr3:uid="{41A36080-1B6C-485A-832F-3023A25C3C09}" name="Disgust" totalsRowFunction="count"/>
+    <tableColumn id="8" xr3:uid="{8FE2A978-974D-4435-833C-9269DC73AD52}" name="Neutral" totalsRowFunction="count"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3275,40 +3465,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K801"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A457" zoomScale="72" workbookViewId="0">
-      <selection activeCell="H476" sqref="H476"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="78" workbookViewId="0">
+      <selection activeCell="B276" sqref="B276"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="42.5546875" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" customWidth="1"/>
+    <col min="7" max="7" width="9" customWidth="1"/>
+    <col min="8" max="8" width="9.44140625" customWidth="1"/>
     <col min="9" max="9" width="16.88671875" customWidth="1"/>
     <col min="10" max="10" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>772</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="7" t="s">
         <v>766</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="7" t="s">
         <v>767</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="7" t="s">
         <v>768</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="7" t="s">
         <v>769</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="7" t="s">
         <v>775</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="7" t="s">
         <v>770</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="7" t="s">
         <v>771</v>
       </c>
       <c r="I1" s="3" t="s">
@@ -5972,7 +6165,7 @@
         <v>0</v>
       </c>
       <c r="H70">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I70" t="str">
         <f t="shared" si="7"/>
@@ -7817,7 +8010,7 @@
         <v>0</v>
       </c>
       <c r="H120">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I120" t="str">
         <f t="shared" si="7"/>
@@ -13531,9 +13724,6 @@
       <c r="G275">
         <v>0</v>
       </c>
-      <c r="H275">
-        <v>1</v>
-      </c>
       <c r="I275" t="str">
         <f t="shared" si="15"/>
         <v>Angry</v>
@@ -31746,21 +31936,74 @@
       </c>
     </row>
     <row r="768" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A768" s="2"/>
+      <c r="A768" s="8" t="s">
+        <v>778</v>
+      </c>
+      <c r="B768">
+        <f>SUBTOTAL(103,Table2[Angry])</f>
+        <v>766</v>
+      </c>
+      <c r="C768">
+        <f>SUBTOTAL(103,Table2[[Sad ]])</f>
+        <v>766</v>
+      </c>
+      <c r="D768">
+        <f ca="1">SUBTOTAL(103,Table2[Happy])</f>
+        <v>58</v>
+      </c>
+      <c r="E768">
+        <f ca="1">SUBTOTAL(103,Table2[Fear])</f>
+        <v>31</v>
+      </c>
+      <c r="F768">
+        <f ca="1">SUBTOTAL(103,Table2[Surprise])</f>
+        <v>31</v>
+      </c>
+      <c r="G768">
+        <f ca="1">SUBTOTAL(103,Table2[Disgust])</f>
+        <v>31</v>
+      </c>
+      <c r="H768">
+        <f ca="1">SUBTOTAL(103,Table2[Neutral])</f>
+        <v>468</v>
+      </c>
+      <c r="I768" s="2"/>
     </row>
     <row r="769" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A769" s="2"/>
-      <c r="B769" s="2"/>
-      <c r="C769" s="2"/>
-      <c r="D769" s="2"/>
-      <c r="E769" s="2"/>
-      <c r="F769" s="2"/>
-      <c r="G769" s="2"/>
-      <c r="H769" s="2"/>
+      <c r="A769" s="5" t="s">
+        <v>778</v>
+      </c>
+      <c r="B769" s="2">
+        <f>COUNTIF(B2:B767,1)</f>
+        <v>59</v>
+      </c>
+      <c r="C769" s="2">
+        <f>COUNTIF(C2:C767,1)</f>
+        <v>49</v>
+      </c>
+      <c r="D769" s="2">
+        <f t="shared" ref="D769:G769" ca="1" si="34">COUNTIF(D2:D767,1)</f>
+        <v>59</v>
+      </c>
+      <c r="E769" s="2">
+        <f t="shared" ca="1" si="34"/>
+        <v>59</v>
+      </c>
+      <c r="F769" s="2">
+        <f t="shared" ca="1" si="34"/>
+        <v>59</v>
+      </c>
+      <c r="G769" s="2">
+        <f t="shared" ca="1" si="34"/>
+        <v>59</v>
+      </c>
+      <c r="H769" s="2">
+        <f ca="1">COUNTIF(H2:H767,1)</f>
+        <v>0</v>
+      </c>
       <c r="I769" s="2"/>
     </row>
     <row r="770" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A770" s="2"/>
       <c r="I770" s="2"/>
     </row>
     <row r="771" spans="1:9" x14ac:dyDescent="0.3">
@@ -31883,24 +32126,58 @@
       <c r="A800" s="2"/>
       <c r="I800" s="2"/>
     </row>
-    <row r="801" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="801" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A801" s="2"/>
-      <c r="I801" s="2"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="K1 K201:K1048576">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="10" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K100">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="9" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K101:K200">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="8" operator="equal">
       <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B767">
+    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C767">
+    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D767">
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E767">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F767">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G767">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H767">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+      <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -32673,5 +32950,8 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId767"/>
+  <tableParts count="1">
+    <tablePart r:id="rId768"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>